<commit_message>
I added the coolest spreadsheet ever
sdfsdf
git kys
git pull
232
</commit_message>
<xml_diff>
--- a/Awesome Spreadsheet.xlsx
+++ b/Awesome Spreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
   <si>
     <t>LOOK AT ALL OF THESE AMAZING NUMBERS GUYS</t>
   </si>
@@ -31,6 +31,48 @@
   </si>
   <si>
     <t>Git hates us all</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>!</t>
   </si>
 </sst>
 </file>
@@ -382,15 +424,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>13</v>
       </c>
@@ -405,7 +447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -413,9 +455,113 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" t="s">
+        <v>7</v>
+      </c>
+      <c r="N8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" t="s">
+        <v>8</v>
+      </c>
+      <c r="N9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>